<commit_message>
Completed projuction files for comm_v0p5
</commit_message>
<xml_diff>
--- a/comm_v0p6/production/rev1/test/BOM_JLCPCB_comm_v0p6_rev1.xlsx
+++ b/comm_v0p6/production/rev1/test/BOM_JLCPCB_comm_v0p6_rev1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -49,25 +49,16 @@
     <t xml:space="preserve">C5137499</t>
   </si>
   <si>
-    <t xml:space="preserve">10uF 25V Aluminum Electrolytic Capacitor</t>
+    <t xml:space="preserve">10uF 50V Multilayer Ceramic Capacitor</t>
   </si>
   <si>
     <t xml:space="preserve">C3</t>
   </si>
   <si>
-    <t xml:space="preserve">SMD,D4xL5.4mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C72484</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22uF 16V Aluminum Electrolytic Capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C72502</t>
+    <t xml:space="preserve">0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2932476</t>
   </si>
   <si>
     <t xml:space="preserve">Conn Header R/A 15pos  2.54mm</t>
@@ -356,7 +347,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -428,10 +419,10 @@
         <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -439,13 +430,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>19</v>
@@ -462,66 +453,50 @@
         <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>